<commit_message>
creates controllers and views. Implements regex
</commit_message>
<xml_diff>
--- a/public/Alumnos.xlsx
+++ b/public/Alumnos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cinthya/Documents/TICs_Cano/etl_school/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A957BA4-9A4F-3946-B3DC-29E4ECC44F81}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D4F377-F45C-294A-9120-4BBACDC35673}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{FCFB9219-B086-8745-9DEB-743660A2A4A8}"/>
+    <workbookView xWindow="840" yWindow="2500" windowWidth="15900" windowHeight="12420" xr2:uid="{FCFB9219-B086-8745-9DEB-743660A2A4A8}"/>
   </bookViews>
   <sheets>
     <sheet name="alumnos" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="111">
   <si>
-    <t>Cristela Aliprando Longo</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -365,6 +362,9 @@
   </si>
   <si>
     <t>progra</t>
+  </si>
+  <si>
+    <t>Cristela2 Aliprando Longo</t>
   </si>
 </sst>
 </file>
@@ -737,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FFB128-0D74-9647-91C3-73FDB7ADF206}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -750,16 +750,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
@@ -767,14 +767,14 @@
         <v>18464471</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="4" t="str">
         <f>CONCATENATE(SUBSTITUTE(B2," ",""),"@Hotmail.com")</f>
-        <v>CristelaAliprandoLongo@Hotmail.com</v>
+        <v>Cristela2AliprandoLongo@Hotmail.com</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.25">
@@ -782,10 +782,10 @@
         <v>15466155</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="4" t="str">
         <f t="shared" ref="D3:D66" si="0">CONCATENATE(SUBSTITUTE(B3," ",""),"@Hotmail.com")</f>
@@ -797,10 +797,10 @@
         <v>17464150</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" si="0"/>
@@ -812,10 +812,10 @@
         <v>18464860</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -827,10 +827,10 @@
         <v>17461591</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -842,10 +842,10 @@
         <v>18464547</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="0"/>
@@ -857,10 +857,10 @@
         <v>16464630</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="4" t="str">
         <f t="shared" si="0"/>
@@ -872,10 +872,10 @@
         <v>17462520</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="4" t="str">
         <f t="shared" si="0"/>
@@ -887,10 +887,10 @@
         <v>16468666</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="0"/>
@@ -902,10 +902,10 @@
         <v>15464018</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="0"/>
@@ -917,10 +917,10 @@
         <v>17467182</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="4" t="str">
         <f t="shared" si="0"/>
@@ -932,10 +932,10 @@
         <v>16469239</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" s="4" t="str">
         <f t="shared" si="0"/>
@@ -947,10 +947,10 @@
         <v>18468225</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="4" t="str">
         <f t="shared" si="0"/>
@@ -962,10 +962,10 @@
         <v>18469085</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" s="4" t="str">
         <f t="shared" si="0"/>
@@ -977,10 +977,10 @@
         <v>18464648</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="4" t="str">
         <f t="shared" si="0"/>
@@ -992,10 +992,10 @@
         <v>15468171</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1007,10 +1007,10 @@
         <v>18465471</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1022,10 +1022,10 @@
         <v>15463701</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1037,10 +1037,10 @@
         <v>18469404</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1052,10 +1052,10 @@
         <v>15465391</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1067,10 +1067,10 @@
         <v>18466684</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1082,10 +1082,10 @@
         <v>18465677</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1097,10 +1097,10 @@
         <v>17468981</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1112,10 +1112,10 @@
         <v>17463277</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1127,10 +1127,10 @@
         <v>18466391</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1142,10 +1142,10 @@
         <v>15469532</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1157,10 +1157,10 @@
         <v>15464364</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1172,10 +1172,10 @@
         <v>16463535</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1187,10 +1187,10 @@
         <v>17467060</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1202,10 +1202,10 @@
         <v>16463355</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1217,10 +1217,10 @@
         <v>16463806</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1232,10 +1232,10 @@
         <v>15469656</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1247,10 +1247,10 @@
         <v>17469898</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1262,10 +1262,10 @@
         <v>18464029</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1277,10 +1277,10 @@
         <v>16465447</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1292,10 +1292,10 @@
         <v>17462800</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D37" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1307,10 +1307,10 @@
         <v>15469187</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D38" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1322,10 +1322,10 @@
         <v>18462234</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1337,10 +1337,10 @@
         <v>18467725</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D40" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1352,10 +1352,10 @@
         <v>16467177</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1367,10 +1367,10 @@
         <v>18466270</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D42" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1382,10 +1382,10 @@
         <v>16469379</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1397,10 +1397,10 @@
         <v>15468580</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1412,10 +1412,10 @@
         <v>18468448</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1427,10 +1427,10 @@
         <v>18468486</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1442,10 +1442,10 @@
         <v>17463150</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1457,10 +1457,10 @@
         <v>18465351</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1472,10 +1472,10 @@
         <v>15467039</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1487,10 +1487,10 @@
         <v>17469961</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1502,10 +1502,10 @@
         <v>15467122</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D51" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1517,10 +1517,10 @@
         <v>16463201</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1532,10 +1532,10 @@
         <v>15466439</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1547,10 +1547,10 @@
         <v>15463178</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1562,10 +1562,10 @@
         <v>16468941</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1577,10 +1577,10 @@
         <v>17468041</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D56" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1592,10 +1592,10 @@
         <v>16467437</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D57" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1607,10 +1607,10 @@
         <v>18466619</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1622,10 +1622,10 @@
         <v>17462765</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1637,10 +1637,10 @@
         <v>17467421</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1652,10 +1652,10 @@
         <v>15469659</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D61" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1667,10 +1667,10 @@
         <v>16464779</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1682,10 +1682,10 @@
         <v>16462553</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1697,10 +1697,10 @@
         <v>15466076</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D64" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1712,10 +1712,10 @@
         <v>16463408</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1727,10 +1727,10 @@
         <v>16461024</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D66" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1742,10 +1742,10 @@
         <v>18468645</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67" s="4" t="str">
         <f t="shared" ref="D67:D101" si="1">CONCATENATE(SUBSTITUTE(B67," ",""),"@Hotmail.com")</f>
@@ -1757,10 +1757,10 @@
         <v>18469255</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D68" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1772,10 +1772,10 @@
         <v>17465213</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D69" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1787,10 +1787,10 @@
         <v>18464274</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D70" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1802,10 +1802,10 @@
         <v>15464352</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D71" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1817,10 +1817,10 @@
         <v>18468089</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D72" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1832,10 +1832,10 @@
         <v>18467364</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D73" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1847,10 +1847,10 @@
         <v>16466944</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1862,10 +1862,10 @@
         <v>17469416</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D75" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1877,10 +1877,10 @@
         <v>17469203</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D76" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1892,10 +1892,10 @@
         <v>15462185</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D77" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1907,10 +1907,10 @@
         <v>16467213</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D78" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1922,10 +1922,10 @@
         <v>17463582</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1937,10 +1937,10 @@
         <v>17469406</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D80" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1952,10 +1952,10 @@
         <v>17468120</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D81" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1967,10 +1967,10 @@
         <v>18461591</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D82" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1982,10 +1982,10 @@
         <v>15461267</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D83" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1997,10 +1997,10 @@
         <v>16467445</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D84" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2012,10 +2012,10 @@
         <v>16466152</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D85" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2027,10 +2027,10 @@
         <v>16469031</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2042,10 +2042,10 @@
         <v>16464673</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D87" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2057,10 +2057,10 @@
         <v>18465532</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D88" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2072,10 +2072,10 @@
         <v>18465580</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D89" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2087,10 +2087,10 @@
         <v>18464018</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D90" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2102,10 +2102,10 @@
         <v>18465773</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D91" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2117,10 +2117,10 @@
         <v>18461009</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D92" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2132,10 +2132,10 @@
         <v>17469471</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D93" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2147,10 +2147,10 @@
         <v>15465421</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D94" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2162,10 +2162,10 @@
         <v>18467934</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D95" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2177,10 +2177,10 @@
         <v>17468681</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D96" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2192,10 +2192,10 @@
         <v>18463553</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D97" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2207,10 +2207,10 @@
         <v>16464956</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D98" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2222,10 +2222,10 @@
         <v>16469445</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D99" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2237,10 +2237,10 @@
         <v>15466671</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D100" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2252,10 +2252,10 @@
         <v>17463028</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D101" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2271,7 +2271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D315775A-CD18-4642-8932-7D47C31872B5}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2279,10 +2279,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" t="s">
         <v>106</v>
-      </c>
-      <c r="B1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2290,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2298,7 +2298,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2306,7 +2306,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>